<commit_message>
magento com produtos compostos e serviços - parcial
</commit_message>
<xml_diff>
--- a/Global/Especificacao/Ambiente/ApiMagento/PedidoMagento/CadastrarPedido/P40_Produtos/P30_CalcularDesconto/Calculo AR CLUBE PREÇO MAGENTO.xlsx
+++ b/Global/Especificacao/Ambiente/ApiMagento/PedidoMagento/CadastrarPedido/P40_Produtos/P30_CalcularDesconto/Calculo AR CLUBE PREÇO MAGENTO.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo.Perez\source\repos\arclube\arclube-trabalhando\arclube\Global\Especificacao\Ambiente\ApiMagento\PedidoMagento\CadastrarPedido\P40_Produtos\P30_CalcularDesconto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositorios\arclube-altera_produtos_compostos_e_frete\arclube\Global\Especificacao\Ambiente\ApiMagento\PedidoMagento\CadastrarPedido\P40_Produtos\P30_CalcularDesconto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0608C0DB-9FDE-436E-A5EB-435CA8FD898E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97593BFE-BB37-4DF7-8F58-E97EE7466C35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{C000D1C8-D7D8-4E83-A17A-82AED5885754}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{C000D1C8-D7D8-4E83-A17A-82AED5885754}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="especificação" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t>QTD</t>
   </si>
@@ -243,16 +243,44 @@
     <t>valor base unitário</t>
   </si>
   <si>
-    <t>PRECISA TIRAR O VALRO DOS SERVIÇOS DO GRAND TOTAL AO RECALCULAR OS VALORES]</t>
+    <t>Precisa tirar o valor dos serviços do grand total ao recalcular os valores</t>
+  </si>
+  <si>
+    <t>PedidoMagentoDto.ListaServicos</t>
+  </si>
+  <si>
+    <t>Descrição 1:</t>
+  </si>
+  <si>
+    <t>Descrição 2:</t>
+  </si>
+  <si>
+    <t>Instalação</t>
+  </si>
+  <si>
+    <t>Reparo da instalação</t>
+  </si>
+  <si>
+    <t>801022</t>
+  </si>
+  <si>
+    <t>801023</t>
+  </si>
+  <si>
+    <t>Auxiliares, sem os serviços:</t>
+  </si>
+  <si>
+    <t>Valores com produtos e serviços somados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -295,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,12 +348,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -336,13 +358,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,11 +399,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Moeda 2" xfId="3" xr:uid="{DBDAFFE4-494F-426F-8A80-70F4D0DA4447}"/>
+    <cellStyle name="Moeda 2 2" xfId="5" xr:uid="{D0867D8B-7232-4B84-90C6-DD55C282CBB1}"/>
+    <cellStyle name="Moeda 3" xfId="4" xr:uid="{8B967138-CCAD-414D-85B9-C5680F50C1FA}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -693,42 +721,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC3154E-6A5D-4698-AC24-EB6D7E840832}">
-  <dimension ref="A2:AE38"/>
+  <dimension ref="A2:AE69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="4.5546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="4.5546875" customWidth="1"/>
-    <col min="19" max="19" width="35.109375" customWidth="1"/>
-    <col min="20" max="20" width="4.5546875" customWidth="1"/>
-    <col min="22" max="22" width="5.5546875" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="4.5703125" customWidth="1"/>
+    <col min="19" max="19" width="35.140625" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" customWidth="1"/>
     <col min="25" max="25" width="12" customWidth="1"/>
-    <col min="26" max="26" width="4.44140625" customWidth="1"/>
+    <col min="26" max="26" width="4.42578125" customWidth="1"/>
     <col min="27" max="30" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="G2" s="22" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G2" s="10" t="s">
         <v>69</v>
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
@@ -748,7 +779,7 @@
       </c>
       <c r="X4" s="21"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="X5" s="10"/>
@@ -760,7 +791,7 @@
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -791,7 +822,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="10"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>33</v>
       </c>
@@ -849,7 +880,7 @@
       </c>
       <c r="AE7" s="10"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -880,7 +911,7 @@
       <c r="AD8" s="10"/>
       <c r="AE8" s="10"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>34</v>
       </c>
@@ -905,7 +936,7 @@
       <c r="AD9" s="10"/>
       <c r="AE9" s="10"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
@@ -918,16 +949,16 @@
       <c r="G10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="22">
         <v>2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="23">
         <v>3000.87</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="23">
         <v>0</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="23">
         <v>12.37</v>
       </c>
       <c r="L10" s="2">
@@ -937,7 +968,7 @@
       <c r="N10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="24">
         <f>+H10+H13</f>
         <v>3</v>
       </c>
@@ -957,7 +988,7 @@
       </c>
       <c r="Y10" s="12">
         <f>+P10*(1-$S$19)</f>
-        <v>1063.197339634801</v>
+        <v>1048.0605595547308</v>
       </c>
       <c r="Z10" s="12"/>
       <c r="AA10" s="12">
@@ -978,7 +1009,7 @@
       </c>
       <c r="AE10" s="10"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>37</v>
       </c>
@@ -988,10 +1019,15 @@
       <c r="D11">
         <v>494.41</v>
       </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="10"/>
       <c r="N11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="24">
         <f>+H10</f>
         <v>2</v>
       </c>
@@ -1015,7 +1051,7 @@
       </c>
       <c r="Y11" s="12">
         <f>+P11*(1-$S$19)</f>
-        <v>455.65731929824557</v>
+        <v>449.17010909090908</v>
       </c>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12">
@@ -1036,11 +1072,16 @@
       </c>
       <c r="AE11" s="10"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="S12" s="8">
-        <f>+I37</f>
-        <v>7078.7199999999984</v>
+        <f>+I36</f>
+        <v>6977.9399999999987</v>
       </c>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
@@ -1054,20 +1095,20 @@
       <c r="AD12" s="12"/>
       <c r="AE12" s="10"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="23">
         <v>1143.6099999999999</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="23">
         <v>0</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="23">
         <v>151.12</v>
       </c>
       <c r="L13" s="2">
@@ -1088,13 +1129,14 @@
       <c r="AD13" s="12"/>
       <c r="AE13" s="10"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="2"/>
       <c r="Q14" s="10"/>
       <c r="S14" s="10" t="s">
@@ -1112,23 +1154,23 @@
       <c r="AD14" s="12"/>
       <c r="AE14" s="10"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="22">
         <v>1</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="23">
         <v>3200.56</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="23">
         <v>0</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="23">
         <v>213.61</v>
       </c>
       <c r="L15" s="2">
@@ -1148,7 +1190,7 @@
       </c>
       <c r="Q15" s="10"/>
       <c r="S15" s="8">
-        <f>+I37-I31+I34</f>
+        <f>+I36-I51+I54</f>
         <v>6967.9399999999987</v>
       </c>
       <c r="U15" s="10"/>
@@ -1163,7 +1205,7 @@
       </c>
       <c r="Y15" s="12">
         <f>+P15*(1-$S$19)</f>
-        <v>1042.2305225921946</v>
+        <v>1027.3922478664192</v>
       </c>
       <c r="Z15" s="12"/>
       <c r="AA15" s="12">
@@ -1184,7 +1226,7 @@
       </c>
       <c r="AE15" s="10"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="N16" s="6" t="s">
         <v>41</v>
@@ -1210,7 +1252,7 @@
       </c>
       <c r="Y16" s="12">
         <f>+P16*(1-$S$19)</f>
-        <v>1935.5828199069097</v>
+        <v>1908.0258552875694</v>
       </c>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12">
@@ -1231,7 +1273,7 @@
       </c>
       <c r="AE16" s="10"/>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -1257,7 +1299,7 @@
       <c r="AD17" s="12"/>
       <c r="AE17" s="10"/>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
@@ -1285,7 +1327,7 @@
       <c r="AD18" s="10"/>
       <c r="AE18" s="10"/>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>41</v>
       </c>
@@ -1297,7 +1339,7 @@
       </c>
       <c r="S19" s="17">
         <f>+(S9-S12)/S9</f>
-        <v>7.8381668456856526E-2</v>
+        <v>9.1502782931354429E-2</v>
       </c>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
@@ -1310,15 +1352,7 @@
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="X20" s="15" t="s">
@@ -1326,7 +1360,7 @@
       </c>
       <c r="Y20" s="13">
         <f>SUMPRODUCT(X8:X19,Y8:Y19)</f>
-        <v>7078.7199999999975</v>
+        <v>6977.94</v>
       </c>
       <c r="Z20" s="13"/>
       <c r="AA20" s="10"/>
@@ -1338,7 +1372,7 @@
       </c>
       <c r="AE20" s="10"/>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="S21" t="s">
         <v>54</v>
       </c>
@@ -1353,14 +1387,15 @@
       <c r="AD21" s="10"/>
       <c r="AE21" s="10"/>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="8">
-        <f>SUM(I8:I19)</f>
-        <v>7345.0399999999991</v>
-      </c>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
       <c r="P22" s="4" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1412,7 @@
       </c>
       <c r="Y22" s="13">
         <f>Y20-AD20</f>
-        <v>110.77999999999793</v>
+        <v>10</v>
       </c>
       <c r="Z22" s="18"/>
       <c r="AA22" s="10"/>
@@ -1386,9 +1421,24 @@
       <c r="AD22" s="10"/>
       <c r="AE22" s="10"/>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G23" t="s">
-        <v>18</v>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="P23" s="4" t="s">
         <v>2</v>
@@ -1408,7 +1458,13 @@
       <c r="AD23" s="10"/>
       <c r="AE23" s="10"/>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
       <c r="P24" t="s">
         <v>47</v>
       </c>
@@ -1428,14 +1484,13 @@
       <c r="AD24" s="10"/>
       <c r="AE24" s="10"/>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="8">
-        <f>SUM(K8:K19)+I34</f>
-        <v>389.77000000000004</v>
-      </c>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
       <c r="P25" t="s">
         <v>48</v>
       </c>
@@ -1456,9 +1511,25 @@
       <c r="AD25" s="10"/>
       <c r="AE25" s="10"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G26" t="s">
-        <v>20</v>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="10">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2">
+        <v>123</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>3.21</v>
+      </c>
+      <c r="L26" s="2">
+        <f>+I26-K26</f>
+        <v>119.79</v>
       </c>
       <c r="P26" t="s">
         <v>46</v>
@@ -1466,8 +1537,8 @@
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="X26" s="8">
-        <f>+Y22-I31+I34</f>
-        <v>-2.0765611452588928E-12</v>
+        <f>+Y22-I51+I54</f>
+        <v>0</v>
       </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
@@ -1477,7 +1548,26 @@
       <c r="AD26" s="10"/>
       <c r="AE26" s="10"/>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>234.57</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>2.31</v>
+      </c>
+      <c r="L27" s="2">
+        <f>+I27-K27</f>
+        <v>232.26</v>
+      </c>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="X27" s="10"/>
@@ -1489,12 +1579,12 @@
       <c r="AD27" s="10"/>
       <c r="AE27" s="10"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G28" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0</v>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
       </c>
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
@@ -1509,14 +1599,18 @@
       <c r="AD28" s="10"/>
       <c r="AE28" s="10"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G29" t="s">
-        <v>22</v>
-      </c>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" t="s">
+        <v>74</v>
+      </c>
+      <c r="L29" s="3"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="X29" s="8">
-        <f>+Y20-I37</f>
+        <f>+Y20-I36</f>
         <v>0</v>
       </c>
       <c r="Y29" s="10"/>
@@ -1527,7 +1621,7 @@
       <c r="AD29" s="10"/>
       <c r="AE29" s="10"/>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
       <c r="X30" s="10"/>
@@ -1539,57 +1633,262 @@
       <c r="AD30" s="10"/>
       <c r="AE30" s="10"/>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G31" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="2">
-        <v>123.45</v>
-      </c>
-      <c r="K31" s="8"/>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
       <c r="X31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="G32" t="s">
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="X32" s="8">
+        <f>+I58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="8">
+        <f>SUM(I8:I21)</f>
+        <v>7345.0399999999991</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="8">
+        <f>SUM(K8:K21)+I54</f>
+        <v>377.1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" s="8">
+        <f>+I34+I51-I35</f>
+        <v>6977.9399999999987</v>
+      </c>
+    </row>
+    <row r="41" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G42" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="8">
+        <f>SUM(I8:I30)</f>
+        <v>7702.6099999999988</v>
+      </c>
+      <c r="J42" s="10"/>
+      <c r="K42" s="8"/>
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G43" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="8">
+        <f>SUM(K8:K30)+I54</f>
+        <v>382.62</v>
+      </c>
+      <c r="J45" s="10"/>
+    </row>
+    <row r="46" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G46" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+    </row>
+    <row r="47" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+    </row>
+    <row r="48" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G48" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" s="10"/>
+      <c r="I48" s="2">
+        <v>0</v>
+      </c>
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G49" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+    </row>
+    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+    </row>
+    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G51" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H51" s="10"/>
+      <c r="I51" s="2">
+        <v>10</v>
+      </c>
+      <c r="J51" s="10"/>
+    </row>
+    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G52" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="X32" s="8">
-        <f>+I38</f>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+    </row>
+    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+    </row>
+    <row r="54" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G54" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H54" s="10"/>
+      <c r="I54" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G34" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="2">
-        <v>12.67</v>
-      </c>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G35" t="s">
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+    </row>
+    <row r="55" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G55" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G37" t="s">
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+    </row>
+    <row r="56" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+    </row>
+    <row r="57" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G57" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I37" s="8">
-        <f>+I22+I31-I25</f>
-        <v>7078.7199999999984</v>
-      </c>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G38" t="s">
+      <c r="H57" s="10"/>
+      <c r="I57" s="8">
+        <f>+I42+I51-I45</f>
+        <v>7329.9899999999989</v>
+      </c>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+    </row>
+    <row r="58" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G58" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="8">
-        <f>SUM(L8:L19)+I31-I34-I37</f>
+      <c r="H58" s="10"/>
+      <c r="I58" s="8">
+        <f>SUM(L8:L30)+I51-I54-I57</f>
         <v>0</v>
       </c>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+    </row>
+    <row r="59" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+    </row>
+    <row r="60" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+    </row>
+    <row r="61" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+    </row>
+    <row r="62" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="K62" s="8"/>
+      <c r="L62" s="10"/>
+    </row>
+    <row r="63" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+    </row>
+    <row r="64" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+    </row>
+    <row r="65" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+    </row>
+    <row r="66" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+    </row>
+    <row r="67" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+    </row>
+    <row r="68" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+    </row>
+    <row r="69" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>